<commit_message>
Final changes done on Leads and Coordinator
</commit_message>
<xml_diff>
--- a/Leads And Coordinator/controller/Codeyuddha participants.xlsx
+++ b/Leads And Coordinator/controller/Codeyuddha participants.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>OFFLINE</t>
+  </si>
+  <si>
+    <t>hetpatel5542@gmail.com</t>
+  </si>
+  <si>
+    <t>7698545581</t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -138,6 +144,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>